<commit_message>
accomodate new params file
</commit_message>
<xml_diff>
--- a/inst/extdata/shiny_parameters.xlsx
+++ b/inst/extdata/shiny_parameters.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/shinycdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061E5292-9F22-3C49-B2EB-5BA3F4B3BB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4F3B73-575E-944A-AD3F-51BDD6646BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="740" windowWidth="27640" windowHeight="16760" activeTab="2" xr2:uid="{76170439-9F00-B945-82EE-6E36AD1655CA}"/>
+    <workbookView xWindow="40" yWindow="740" windowWidth="17780" windowHeight="16760" activeTab="3" xr2:uid="{76170439-9F00-B945-82EE-6E36AD1655CA}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="2" r:id="rId1"/>
     <sheet name="crosstabs" sheetId="3" r:id="rId2"/>
     <sheet name="graphs" sheetId="1" r:id="rId3"/>
+    <sheet name="labels" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="490">
   <si>
     <t>Q1_0</t>
   </si>
@@ -1007,13 +1008,514 @@
   </si>
   <si>
     <t>23. Assessment of Drought Response - Non-Delta Californians</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>Civic Engagement &amp; Governance</t>
+  </si>
+  <si>
+    <t>Sense of Place</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Quality of Life</t>
+  </si>
+  <si>
+    <t>Risk and Resilience to Climate Change</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>None of these</t>
+  </si>
+  <si>
+    <t>Live in or near the Delta region</t>
+  </si>
+  <si>
+    <t>Work in the Delta</t>
+  </si>
+  <si>
+    <t>Visit the Delta for fun or recreation</t>
+  </si>
+  <si>
+    <t>Farm in the Delta</t>
+  </si>
+  <si>
+    <t>Commute through the Delta</t>
+  </si>
+  <si>
+    <t>None of the above</t>
+  </si>
+  <si>
+    <t>I am proud to live in the Delta.</t>
+  </si>
+  <si>
+    <t>I feel attached to the natural environment of the Delta.</t>
+  </si>
+  <si>
+    <t>I depend on the Delta for my job or livelihood.</t>
+  </si>
+  <si>
+    <t>I depend on fishing or gathering in the Delta as a source of food.</t>
+  </si>
+  <si>
+    <t>I have a sense of responsibility  toward the Delta.</t>
+  </si>
+  <si>
+    <t>I enjoy doing outdoor recreational activities in the Delta.</t>
+  </si>
+  <si>
+    <t>I have familial, cultural, or historical ties to the Delta.</t>
+  </si>
+  <si>
+    <t>My family has lived in the Delta for more than one generation.</t>
+  </si>
+  <si>
+    <t>The Delta is not important to me.</t>
+  </si>
+  <si>
+    <t>The Delta is an important ecosystem.</t>
+  </si>
+  <si>
+    <t>The Delta is a good region for outdoor recreation.</t>
+  </si>
+  <si>
+    <t>The Delta is a place of cultural and historical importance.</t>
+  </si>
+  <si>
+    <t>The Delta is an important agricultural region for the state.</t>
+  </si>
+  <si>
+    <t>Please tell us which of the following apply to you. Do you currently...? Select all that apply.</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>Which of the following statements describe YOUR relationship to the Delta? Select all that apply.</t>
+  </si>
+  <si>
+    <t>Which of the following statements describe why YOU feel the Delta is important? Select all that apply.</t>
+  </si>
+  <si>
+    <t>The Delta is important as California's water hub.</t>
+  </si>
+  <si>
+    <t>The following are some factors that people value about living in the Delta. Which factors, if any, do you personally value most about living in the Delta area? Select up to three.</t>
+  </si>
+  <si>
+    <t>How long have you personally lived in or near the Delta region? Please provide the length of time in years. If you have lived in or near the Delta region for less than one year, please round up to 1.</t>
+  </si>
+  <si>
+    <t>Which best describes the area where you live?</t>
+  </si>
+  <si>
+    <t>Access to outdoor recreation opportunities</t>
+  </si>
+  <si>
+    <t>Access to waterways and waterfronts</t>
+  </si>
+  <si>
+    <t>Agricultural region</t>
+  </si>
+  <si>
+    <t>Close proximity between urban and rural areas</t>
+  </si>
+  <si>
+    <t>Historic and culturally significant areas</t>
+  </si>
+  <si>
+    <t>Quiet and solitude</t>
+  </si>
+  <si>
+    <t>Scenic beauty</t>
+  </si>
+  <si>
+    <t>Sense of community</t>
+  </si>
+  <si>
+    <t>Other. Please specify</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of these are things I value about living near the Delta  </t>
+  </si>
+  <si>
+    <t>The following are some factors that present potential challenges to the well-being of Delta residents. Please select which factors, if any, present the largest challenges to your personal well-being as a Delta resident.</t>
+  </si>
+  <si>
+    <t>None of these are challenging for my personal well-being</t>
+  </si>
+  <si>
+    <t>Affordability of basic needs (e.g., housing, food, healthcare)</t>
+  </si>
+  <si>
+    <t>Access to highspeed internet</t>
+  </si>
+  <si>
+    <t>Aging infrastructure (e.g., roads, levees, bridges)</t>
+  </si>
+  <si>
+    <t>Climate change/Global warming</t>
+  </si>
+  <si>
+    <t>Delta Conveyance/Delta Tunnel projects</t>
+  </si>
+  <si>
+    <t>Environmental decline</t>
+  </si>
+  <si>
+    <t>Lack of job or education opportunities</t>
+  </si>
+  <si>
+    <t>Threats to public safety (e.g., first responders, trespassing, vandalis</t>
+  </si>
+  <si>
+    <t>Social inequality</t>
+  </si>
+  <si>
+    <t>Traffic congestion/Limited transportation options</t>
+  </si>
+  <si>
+    <t>Urban/Suburban development</t>
+  </si>
+  <si>
+    <t>Other.</t>
+  </si>
+  <si>
+    <t>Do you engage in any of the following activities in the Delta? Select all that apply.</t>
+  </si>
+  <si>
+    <t>Wildlife viewing/Birding</t>
+  </si>
+  <si>
+    <t>Fishing or hunting</t>
+  </si>
+  <si>
+    <t>Water-based activities (e.g., boat, kayak/canoe, swim)</t>
+  </si>
+  <si>
+    <t>Land-based activities (e.g., walk, hike, bicycle, camp, picnic)</t>
+  </si>
+  <si>
+    <t>Attend/Visit cultural events, festivals, or historical places</t>
+  </si>
+  <si>
+    <t>Spiritual or religious practices or rituals related to the Delta environment</t>
+  </si>
+  <si>
+    <t>Who do you feel best advocates for your interests in the Delta? (For example, this could be a community organization or group, a public official, a government entity, a local leader, etc.)</t>
+  </si>
+  <si>
+    <t>Please rate your overall level of satisfaction with your quality of life in the Delta.</t>
+  </si>
+  <si>
+    <t>Have you or anyone in your home experienced any of the following impacts while living in the Delta? Select all that apply.</t>
+  </si>
+  <si>
+    <t>Flooded property (e.g., home, farm, roadway)</t>
+  </si>
+  <si>
+    <t>Well failure or contamination</t>
+  </si>
+  <si>
+    <t>Natural disaster (e.g., flood, wildfire, earthquake, drought, etc.)</t>
+  </si>
+  <si>
+    <t>Moved/Relocated due to disaster</t>
+  </si>
+  <si>
+    <t>Excessive heat</t>
+  </si>
+  <si>
+    <t>Worsening air quality</t>
+  </si>
+  <si>
+    <t>Worsening water quality</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>How concerned are you about each of the following environmental changes affecting the Delta over the next 25 years?</t>
+  </si>
+  <si>
+    <t>Rising sea levels</t>
+  </si>
+  <si>
+    <t>More frequent/severe heat waves</t>
+  </si>
+  <si>
+    <t>More frequent/severe droughts</t>
+  </si>
+  <si>
+    <t>More frequent/severe floods</t>
+  </si>
+  <si>
+    <t>More frequent/severe wildfires and smoke</t>
+  </si>
+  <si>
+    <t>Are there any other environmental changes not mentioned above that you are concerned about affecting the Delta?</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Do you believe climate change is caused...</t>
+  </si>
+  <si>
+    <t>How much do you think the environmental changes mentioned above (e.g. rising sea levels, heat waves, droughts, floods, wildfires, worsening air and water quality, etc.) are a result of climate change?</t>
+  </si>
+  <si>
+    <t>To prepare for possible environmental and climate change impacts to the Delta, would you support policies that led to any of the following actions? Select all that apply.</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>You pay an annual fee for local levee improvements to reduce flood risk</t>
+  </si>
+  <si>
+    <t>You pay an annual fee to fund a local district to be responsible for climate ri</t>
+  </si>
+  <si>
+    <t>State government dedicates more land to restoring wildlife habitat</t>
+  </si>
+  <si>
+    <t>State or local government increases public access to parks, trails, or open spa</t>
+  </si>
+  <si>
+    <t>State government dedicates more funding for sustainable agriculture</t>
+  </si>
+  <si>
+    <t>State government mandates decreases in farmland during drought years to save wa</t>
+  </si>
+  <si>
+    <t>State government dedicates more water to agriculture</t>
+  </si>
+  <si>
+    <t>State government dedicates more water to the environment</t>
+  </si>
+  <si>
+    <t>State government dedicates more water to cities and communities</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19a</t>
+  </si>
+  <si>
+    <t>19b</t>
+  </si>
+  <si>
+    <t>Are there any other actions (not listed above) that you would like to see taken to prepare the Delta for possible environmental and climate change impacts?</t>
+  </si>
+  <si>
+    <t>California is currently in a severe drought.</t>
+  </si>
+  <si>
+    <t>California should be preparing for more severe droughts in the future.</t>
+  </si>
+  <si>
+    <t>Have you personally experienced drought impacts directly? If so, how?</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>In response to the current drought in California, would you say state and local governments are...</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>In response to the current drought in California, would you say other people living in the Delta are...</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>In response to the current drought in California, would you say  other Californians living OUTSIDE of the Delta are...</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Which of the following resources do you currently have access to? Select all that apply.</t>
+  </si>
+  <si>
+    <t>Air conditioned or climate-controlled environment</t>
+  </si>
+  <si>
+    <t>Air filters</t>
+  </si>
+  <si>
+    <t>Backup power supply/Generator</t>
+  </si>
+  <si>
+    <t>Personal computer with internet connection</t>
+  </si>
+  <si>
+    <t>Mobile device with internet connection</t>
+  </si>
+  <si>
+    <t>Domestic well for drinking water</t>
+  </si>
+  <si>
+    <t>Sewage system</t>
+  </si>
+  <si>
+    <t>Homeowner's or renter's insurance</t>
+  </si>
+  <si>
+    <t>Flood insurance</t>
+  </si>
+  <si>
+    <t>Earthquake insurance</t>
+  </si>
+  <si>
+    <t>Health insurance</t>
+  </si>
+  <si>
+    <t>Personal motorized vehicle such as car, truck, motorbike, etc.</t>
+  </si>
+  <si>
+    <t>Public transportation such as bus or train route</t>
+  </si>
+  <si>
+    <t>Emergency financial resources (e.g., savings, credit, loans)</t>
+  </si>
+  <si>
+    <t>Family, friends, or supportive community you could stay with in the case of an emergency event evacuation</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Which best describes your political views?</t>
+  </si>
+  <si>
+    <t>Thank you for completing this survey! Before you go, we are testing out four more questions to use on future surveys. Would you be able to answer a few more quick questions before going?</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Please rate the following entities on how much you trust them to act in the best interests of the Delta.</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>Federal policy makers</t>
+  </si>
+  <si>
+    <t>State policy makers</t>
+  </si>
+  <si>
+    <t>Local policy makers</t>
+  </si>
+  <si>
+    <t>Scientific experts</t>
+  </si>
+  <si>
+    <t>Community advisory groups</t>
+  </si>
+  <si>
+    <t>Local residents</t>
+  </si>
+  <si>
+    <t>How likely are you to get involved in any of the following ways for a Delta issue that is important to you?</t>
+  </si>
+  <si>
+    <t>Attending/participating in a hearing or public meeting</t>
+  </si>
+  <si>
+    <t>Attending/Participating in a demonstration</t>
+  </si>
+  <si>
+    <t>Volunteering with an advocacy group</t>
+  </si>
+  <si>
+    <t>Writing a blog or letter to a newspaper</t>
+  </si>
+  <si>
+    <t>Calling or writing a letter to an elected official or public agency</t>
+  </si>
+  <si>
+    <t>Signing a petition</t>
+  </si>
+  <si>
+    <t>Voting in an election</t>
+  </si>
+  <si>
+    <t>Taking a job that allows me to work on the issue</t>
+  </si>
+  <si>
+    <t>Is there another way that was not listed above that you would be likely to get involved in the Delta for an issue that mattered to you?</t>
+  </si>
+  <si>
+    <t>Are any of the following factors barriers to engaging with issues facing the Delta? Select all that apply.</t>
+  </si>
+  <si>
+    <t>I am unfamiliar with the issues.</t>
+  </si>
+  <si>
+    <t>I feel like my perspective is not represented.</t>
+  </si>
+  <si>
+    <t>I feel like my input will not affect decision-making.</t>
+  </si>
+  <si>
+    <t>I don't know how or when to engage.</t>
+  </si>
+  <si>
+    <t>I am unable to get to meetings (e.g., transportation; location or time are inconvenient).</t>
+  </si>
+  <si>
+    <t>I do not have internet or technology access to attend virtual meetings.</t>
+  </si>
+  <si>
+    <t>I am too busy with other obligations and priorities.</t>
+  </si>
+  <si>
+    <t>COVID-related impacts (e.g., health, time, financial resources or obligations).</t>
+  </si>
+  <si>
+    <t>I am not interested in the issues.</t>
+  </si>
+  <si>
+    <t>Other barrier. Please specify</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1034,13 +1536,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1055,7 +1569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1064,6 +1578,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3149,10 +3673,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5370D6F9-7760-C640-A095-DECD66441409}">
-  <dimension ref="A1:C147"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3160,9 +3684,10 @@
     <col min="1" max="1" width="27.5" customWidth="1"/>
     <col min="2" max="2" width="57.83203125" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="39.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>147</v>
       </c>
@@ -3172,8 +3697,11 @@
       <c r="C1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3183,8 +3711,11 @@
       <c r="C2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3194,8 +3725,11 @@
       <c r="C3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3205,8 +3739,11 @@
       <c r="C4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3216,8 +3753,11 @@
       <c r="C5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3227,8 +3767,11 @@
       <c r="C6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3238,8 +3781,11 @@
       <c r="C7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3250,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3260,8 +3806,11 @@
       <c r="C9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3271,8 +3820,11 @@
       <c r="C10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3282,8 +3834,11 @@
       <c r="C11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3293,8 +3848,11 @@
       <c r="C12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3304,8 +3862,11 @@
       <c r="C13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3315,8 +3876,11 @@
       <c r="C14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3326,8 +3890,11 @@
       <c r="C15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3337,8 +3904,11 @@
       <c r="C16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3348,8 +3918,11 @@
       <c r="C17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3359,8 +3932,11 @@
       <c r="C18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3370,8 +3946,11 @@
       <c r="C19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3381,8 +3960,11 @@
       <c r="C20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3392,8 +3974,11 @@
       <c r="C21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -3403,8 +3988,11 @@
       <c r="C22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -3414,8 +4002,11 @@
       <c r="C23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3425,8 +4016,11 @@
       <c r="C24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3437,7 +4031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3447,8 +4041,11 @@
       <c r="C26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3458,8 +4055,11 @@
       <c r="C27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3469,8 +4069,11 @@
       <c r="C28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -3480,8 +4083,11 @@
       <c r="C29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -3491,8 +4097,11 @@
       <c r="C30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3502,8 +4111,11 @@
       <c r="C31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3513,8 +4125,11 @@
       <c r="C32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -3524,8 +4139,11 @@
       <c r="C33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -3535,8 +4153,11 @@
       <c r="C34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3546,8 +4167,11 @@
       <c r="C35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -3557,8 +4181,11 @@
       <c r="C36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -3568,8 +4195,11 @@
       <c r="C37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -3579,8 +4209,11 @@
       <c r="C38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -3590,8 +4223,11 @@
       <c r="C39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -3601,8 +4237,11 @@
       <c r="C40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -3612,8 +4251,11 @@
       <c r="C41" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -3623,8 +4265,11 @@
       <c r="C42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -3634,8 +4279,11 @@
       <c r="C43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -3645,8 +4293,11 @@
       <c r="C44" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -3656,8 +4307,11 @@
       <c r="C45" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -3667,8 +4321,11 @@
       <c r="C46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -3678,8 +4335,11 @@
       <c r="C47" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -3690,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -3700,8 +4360,11 @@
       <c r="C49" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -3711,8 +4374,11 @@
       <c r="C50" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -3722,8 +4388,11 @@
       <c r="C51" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -3733,8 +4402,11 @@
       <c r="C52" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -3744,8 +4416,11 @@
       <c r="C53" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -3755,8 +4430,11 @@
       <c r="C54" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -3766,8 +4444,11 @@
       <c r="C55" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -3778,7 +4459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3788,8 +4469,11 @@
       <c r="C57" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -3800,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -3810,8 +4494,11 @@
       <c r="C59" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -3821,8 +4508,11 @@
       <c r="C60" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -3832,8 +4522,11 @@
       <c r="C61" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -3843,8 +4536,11 @@
       <c r="C62" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -3854,8 +4550,11 @@
       <c r="C63" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -3865,8 +4564,11 @@
       <c r="C64" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -3876,8 +4578,11 @@
       <c r="C65" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -3887,8 +4592,11 @@
       <c r="C66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -3898,8 +4606,11 @@
       <c r="C67" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -3909,8 +4620,11 @@
       <c r="C68" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -3920,8 +4634,11 @@
       <c r="C69" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -3931,8 +4648,11 @@
       <c r="C70" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -3942,8 +4662,11 @@
       <c r="C71" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -3953,8 +4676,11 @@
       <c r="C72" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -3964,8 +4690,11 @@
       <c r="C73" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -3975,8 +4704,11 @@
       <c r="C74" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -3986,8 +4718,11 @@
       <c r="C75" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -3997,8 +4732,11 @@
       <c r="C76" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -4008,8 +4746,11 @@
       <c r="C77" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -4019,8 +4760,11 @@
       <c r="C78" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -4030,8 +4774,11 @@
       <c r="C79" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -4041,8 +4788,11 @@
       <c r="C80" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -4052,8 +4802,11 @@
       <c r="C81" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -4063,8 +4816,11 @@
       <c r="C82" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -4074,8 +4830,11 @@
       <c r="C83" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -4085,8 +4844,11 @@
       <c r="C84" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -4096,8 +4858,11 @@
       <c r="C85" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -4107,8 +4872,11 @@
       <c r="C86" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -4119,7 +4887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -4129,8 +4897,11 @@
       <c r="C88" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -4140,8 +4911,11 @@
       <c r="C89" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -4151,8 +4925,11 @@
       <c r="C90" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -4162,8 +4939,11 @@
       <c r="C91" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -4173,8 +4953,11 @@
       <c r="C92" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -4184,8 +4967,11 @@
       <c r="C93" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -4195,8 +4981,11 @@
       <c r="C94" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -4206,8 +4995,11 @@
       <c r="C95" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -4217,8 +5009,11 @@
       <c r="C96" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -4228,8 +5023,11 @@
       <c r="C97" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -4239,8 +5037,11 @@
       <c r="C98" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -4250,8 +5051,11 @@
       <c r="C99" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -4261,8 +5065,11 @@
       <c r="C100" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -4272,8 +5079,11 @@
       <c r="C101" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -4283,8 +5093,11 @@
       <c r="C102" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -4294,8 +5107,11 @@
       <c r="C103" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -4305,8 +5121,11 @@
       <c r="C104" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -4316,8 +5135,11 @@
       <c r="C105" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -4327,8 +5149,11 @@
       <c r="C106" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -4338,8 +5163,11 @@
       <c r="C107" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -4349,8 +5177,11 @@
       <c r="C108" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -4360,8 +5191,11 @@
       <c r="C109" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -4371,8 +5205,11 @@
       <c r="C110" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -4383,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -4393,8 +5230,11 @@
       <c r="C112" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D112" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -4404,8 +5244,11 @@
       <c r="C113" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -4415,8 +5258,11 @@
       <c r="C114" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -4426,8 +5272,11 @@
       <c r="C115" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D115" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -4437,8 +5286,11 @@
       <c r="C116" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -4448,8 +5300,11 @@
       <c r="C117" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -4459,8 +5314,11 @@
       <c r="C118" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -4470,8 +5328,11 @@
       <c r="C119" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -4481,8 +5342,11 @@
       <c r="C120" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D120" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -4492,8 +5356,11 @@
       <c r="C121" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -4503,8 +5370,11 @@
       <c r="C122" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -4514,8 +5384,11 @@
       <c r="C123" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -4525,8 +5398,11 @@
       <c r="C124" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -4536,8 +5412,11 @@
       <c r="C125" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -4548,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -4558,8 +5437,11 @@
       <c r="C127" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -4569,8 +5451,11 @@
       <c r="C128" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -4580,8 +5465,11 @@
       <c r="C129" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -4591,8 +5479,11 @@
       <c r="C130" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -4602,8 +5493,11 @@
       <c r="C131" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -4613,8 +5507,11 @@
       <c r="C132" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -4624,8 +5521,11 @@
       <c r="C133" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -4635,8 +5535,11 @@
       <c r="C134" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D134" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -4647,7 +5550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -4657,8 +5560,11 @@
       <c r="C136" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -4668,8 +5574,11 @@
       <c r="C137" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D137" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
@@ -4679,8 +5588,11 @@
       <c r="C138" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
@@ -4691,7 +5603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -4701,8 +5613,11 @@
       <c r="C140" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -4712,8 +5627,11 @@
       <c r="C141" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -4723,8 +5641,11 @@
       <c r="C142" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -4734,8 +5655,11 @@
       <c r="C143" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -4745,8 +5669,11 @@
       <c r="C144" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D144" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -4756,8 +5683,11 @@
       <c r="C145" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -4767,8 +5697,11 @@
       <c r="C146" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -4778,13 +5711,1250 @@
       <c r="C147" t="b">
         <v>1</v>
       </c>
+      <c r="D147" t="s">
+        <v>326</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="D1 C1:C1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB6DCF2-FCCB-AD4E-AF28-32832A048715}">
+  <dimension ref="A1:D135"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="7"/>
+    <col min="3" max="3" width="70" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.1640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7">
+        <v>8</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7">
+        <v>9</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7">
+        <v>10</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="7">
+        <v>12</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="7">
+        <v>13</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected errors, and also added some metadata for xt
</commit_message>
<xml_diff>
--- a/inst/extdata/shiny_parameters.xlsx
+++ b/inst/extdata/shiny_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/shinycdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1ED394B-06E7-E946-B08A-A97B2C99D2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584388BF-5458-084C-B8C3-80CA0577BE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="740" windowWidth="28480" windowHeight="18180" activeTab="2" xr2:uid="{76170439-9F00-B945-82EE-6E36AD1655CA}"/>
+    <workbookView xWindow="7140" yWindow="740" windowWidth="21340" windowHeight="18180" activeTab="1" xr2:uid="{76170439-9F00-B945-82EE-6E36AD1655CA}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="681">
   <si>
     <t>Q1_0</t>
   </si>
@@ -1817,22 +1817,366 @@
   <si>
     <t>This website provides an easy-to-navigate tool for exploring the data from the 2023 Delta Residents Survey. Keep reading for more information about the survey or use the tabs at the top of this page to navigate to explore survey results in graphs, tables, and maps. A full report of all survey results can be found &lt;a href='https://www.openicpsr.org/openicpsr/project/195447/version/V2/view?path=/openicpsr/195447/fcr:versions/V2/2023-DRS-Results-Summary-Report.pdf&amp;type=file' target = "_blank" class="accordion-link"&gt;here&lt;/a&gt;.</t>
   </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Resident</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>Recreation</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
+    <t>Commute</t>
+  </si>
+  <si>
+    <t>Pride</t>
+  </si>
+  <si>
+    <t>Env attachment</t>
+  </si>
+  <si>
+    <t>Livelihood</t>
+  </si>
+  <si>
+    <t>Subsistence</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>Cultural</t>
+  </si>
+  <si>
+    <t>Generational</t>
+  </si>
+  <si>
+    <t>Unimportant</t>
+  </si>
+  <si>
+    <t>Ecological</t>
+  </si>
+  <si>
+    <t>Recreational</t>
+  </si>
+  <si>
+    <t>Agricultural</t>
+  </si>
+  <si>
+    <t>Hydrological</t>
+  </si>
+  <si>
+    <t>Recreational access</t>
+  </si>
+  <si>
+    <t>Waterfront access</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Urban proximity</t>
+  </si>
+  <si>
+    <t>Cultural significance</t>
+  </si>
+  <si>
+    <t>Tranquility</t>
+  </si>
+  <si>
+    <t>Beauty</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Basic needs</t>
+  </si>
+  <si>
+    <t>Delta Conveyance</t>
+  </si>
+  <si>
+    <t>Env decline</t>
+  </si>
+  <si>
+    <t>Job opportunities</t>
+  </si>
+  <si>
+    <t>Public safety</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Urb development</t>
+  </si>
+  <si>
+    <t>Internet access</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>Climate change</t>
+  </si>
+  <si>
+    <t>Wildlife viewing</t>
+  </si>
+  <si>
+    <t>Water recreation</t>
+  </si>
+  <si>
+    <t>Land recreation</t>
+  </si>
+  <si>
+    <t>Cultural events</t>
+  </si>
+  <si>
+    <t>Spiritual</t>
+  </si>
+  <si>
+    <t>Life Satisfaction</t>
+  </si>
+  <si>
+    <t>Flooded property</t>
+  </si>
+  <si>
+    <t>Well outage</t>
+  </si>
+  <si>
+    <t>Disaster</t>
+  </si>
+  <si>
+    <t>Disaster-relocation</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
+    <t>Air quality</t>
+  </si>
+  <si>
+    <t>Water quality</t>
+  </si>
+  <si>
+    <t>Sea level rise</t>
+  </si>
+  <si>
+    <t>Heat waves</t>
+  </si>
+  <si>
+    <t>Droughts</t>
+  </si>
+  <si>
+    <t>Floods</t>
+  </si>
+  <si>
+    <t>Wildfire-smoke</t>
+  </si>
+  <si>
+    <t>Levee fee</t>
+  </si>
+  <si>
+    <t>Hazard abatement district</t>
+  </si>
+  <si>
+    <t>Wildlife restoration</t>
+  </si>
+  <si>
+    <t>Open spaces</t>
+  </si>
+  <si>
+    <t>Sustainable agriculture</t>
+  </si>
+  <si>
+    <t>Fallow farmland</t>
+  </si>
+  <si>
+    <t>Water for agriculture</t>
+  </si>
+  <si>
+    <t>Water for environment</t>
+  </si>
+  <si>
+    <t>Water for cities</t>
+  </si>
+  <si>
+    <t>Currently in a drought</t>
+  </si>
+  <si>
+    <t>Preparing for more severe droughts</t>
+  </si>
+  <si>
+    <t>21. Assessment of Drought Response</t>
+  </si>
+  <si>
+    <t>State and local government</t>
+  </si>
+  <si>
+    <t>22. Assessment of Drought Response</t>
+  </si>
+  <si>
+    <t>Other residents</t>
+  </si>
+  <si>
+    <t>23. Assessment of Drought Response</t>
+  </si>
+  <si>
+    <t>Non-Delta Californians</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Home insurance</t>
+  </si>
+  <si>
+    <t>Personal vehicle</t>
+  </si>
+  <si>
+    <t>Public transit</t>
+  </si>
+  <si>
+    <t>Emergency finances</t>
+  </si>
+  <si>
+    <t>Emergency accomodations</t>
+  </si>
+  <si>
+    <t>Backup power</t>
+  </si>
+  <si>
+    <t>Computer internet</t>
+  </si>
+  <si>
+    <t>Mobile internet</t>
+  </si>
+  <si>
+    <t>Drinking well</t>
+  </si>
+  <si>
+    <t>Sewage</t>
+  </si>
+  <si>
+    <t>Scientists</t>
+  </si>
+  <si>
+    <t>Community groups</t>
+  </si>
+  <si>
+    <t>Public meeting participation</t>
+  </si>
+  <si>
+    <t>Demonstrations</t>
+  </si>
+  <si>
+    <t>Advocacy group volunteering</t>
+  </si>
+  <si>
+    <t>Editorial writing</t>
+  </si>
+  <si>
+    <t>Writing government</t>
+  </si>
+  <si>
+    <t>Sign petition</t>
+  </si>
+  <si>
+    <t>Voting</t>
+  </si>
+  <si>
+    <t>Issue-based employment</t>
+  </si>
+  <si>
+    <t>Unfamiliarity</t>
+  </si>
+  <si>
+    <t>Unrepresented</t>
+  </si>
+  <si>
+    <t>Ineffectual input</t>
+  </si>
+  <si>
+    <t>Uncertain how to engage</t>
+  </si>
+  <si>
+    <t>Meetings inaccessible</t>
+  </si>
+  <si>
+    <t>No virtual access</t>
+  </si>
+  <si>
+    <t>Too busy</t>
+  </si>
+  <si>
+    <t>No Preferred Language</t>
+  </si>
+  <si>
+    <t>COVID impacts</t>
+  </si>
+  <si>
+    <t>Disinterested</t>
+  </si>
+  <si>
+    <t>full_response</t>
+  </si>
+  <si>
+    <t>I have a sense of responsibility toward the Delta.</t>
+  </si>
+  <si>
+    <t>None of these are things I value about living near the Delta.</t>
+  </si>
+  <si>
+    <t>Other. Please specify:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You pay an annual fee to fund a local district to be responsible for climate risk reduction (for example, the Delta Region Geological Hazard Abatement District in Isleton)  </t>
+  </si>
+  <si>
+    <t>State or local government increases public access to parks, trails, or open spaces</t>
+  </si>
+  <si>
+    <t>State government mandates decreases in farmland during drought years to save water (i.e. fallow farm land)</t>
+  </si>
+  <si>
+    <t>Agreement that California is in an extreme drought</t>
+  </si>
+  <si>
+    <t>Agreement that California should be preparing for more severe droughts in the future</t>
+  </si>
+  <si>
+    <t>Another way that was not listed above</t>
+  </si>
+  <si>
+    <t>My preferred language is not available (e.g., no translation or interpretation is available).</t>
+  </si>
+  <si>
+    <t>Other barrier. Please specify:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1890,12 +2234,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1906,13 +2249,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1920,6 +2283,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3451,14 +3824,14 @@
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E73" s="7"/>
+      <c r="E73" s="6"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E74" s="8"/>
+      <c r="E74" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3469,18 +3842,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B35F82-DAC3-AF45-8FCA-85CC06C5BE17}">
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="70.33203125" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>147</v>
       </c>
@@ -3490,8 +3866,17 @@
       <c r="C1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E1" t="s">
+        <v>565</v>
+      </c>
+      <c r="F1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>187</v>
       </c>
@@ -3501,8 +3886,11 @@
       <c r="C2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>188</v>
       </c>
@@ -3512,8 +3900,11 @@
       <c r="C3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3523,9 +3914,17 @@
       <c r="C4" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" t="s">
+        <v>566</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3535,9 +3934,17 @@
       <c r="C5" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" t="s">
+        <v>567</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -3547,9 +3954,17 @@
       <c r="C6" t="b">
         <v>1</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>568</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3559,9 +3974,17 @@
       <c r="C7" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" t="s">
+        <v>569</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3571,9 +3994,17 @@
       <c r="C8" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" t="s">
+        <v>570</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -3583,9 +4014,17 @@
       <c r="C9" t="b">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" t="s">
+        <v>571</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -3595,8 +4034,11 @@
       <c r="C10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3606,8 +4048,11 @@
       <c r="C11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3617,8 +4062,17 @@
       <c r="C12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" t="s">
+        <v>566</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -3628,8 +4082,17 @@
       <c r="C13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" t="s">
+        <v>572</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -3639,8 +4102,17 @@
       <c r="C14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" t="s">
+        <v>573</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -3650,8 +4122,17 @@
       <c r="C15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" t="s">
+        <v>574</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3661,8 +4142,17 @@
       <c r="C16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" t="s">
+        <v>575</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -3672,8 +4162,17 @@
       <c r="C17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" t="s">
+        <v>576</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -3683,8 +4182,17 @@
       <c r="C18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" t="s">
+        <v>569</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -3694,8 +4202,17 @@
       <c r="C19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E19" t="s">
+        <v>577</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -3705,8 +4222,17 @@
       <c r="C20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" t="s">
+        <v>578</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -3716,8 +4242,17 @@
       <c r="C21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" t="s">
+        <v>579</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -3727,8 +4262,17 @@
       <c r="C22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" t="s">
+        <v>580</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -3738,8 +4282,17 @@
       <c r="C23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" t="s">
+        <v>581</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -3749,8 +4302,17 @@
       <c r="C24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" t="s">
+        <v>577</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -3760,8 +4322,17 @@
       <c r="C25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" t="s">
+        <v>582</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -3771,8 +4342,17 @@
       <c r="C26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" t="s">
+        <v>583</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -3782,8 +4362,11 @@
       <c r="C27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3793,8 +4376,17 @@
       <c r="C28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" t="s">
+        <v>566</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3804,8 +4396,17 @@
       <c r="C29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" t="s">
+        <v>584</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3815,8 +4416,17 @@
       <c r="C30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>164</v>
+      </c>
+      <c r="E30" t="s">
+        <v>585</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -3826,8 +4436,17 @@
       <c r="C31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" t="s">
+        <v>586</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3837,8 +4456,17 @@
       <c r="C32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>164</v>
+      </c>
+      <c r="E32" t="s">
+        <v>587</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3848,8 +4476,17 @@
       <c r="C33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>164</v>
+      </c>
+      <c r="E33" t="s">
+        <v>588</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3859,8 +4496,17 @@
       <c r="C34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>164</v>
+      </c>
+      <c r="E34" t="s">
+        <v>589</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3870,8 +4516,17 @@
       <c r="C35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" t="s">
+        <v>590</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3881,8 +4536,17 @@
       <c r="C36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>164</v>
+      </c>
+      <c r="E36" t="s">
+        <v>591</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3892,8 +4556,17 @@
       <c r="C37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37" t="s">
+        <v>592</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3903,8 +4576,17 @@
       <c r="C38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" t="s">
+        <v>566</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3914,129 +4596,237 @@
       <c r="C39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" t="s">
+        <v>593</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="C40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" t="s">
+        <v>600</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C41" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>165</v>
+      </c>
+      <c r="E41" t="s">
+        <v>601</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>165</v>
+      </c>
+      <c r="E42" t="s">
+        <v>602</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" t="s">
+        <v>594</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C44" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" t="s">
+        <v>595</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" t="s">
+        <v>596</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>165</v>
+      </c>
+      <c r="E46" t="s">
+        <v>597</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C47" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" t="s">
+        <v>372</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C48" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" t="s">
+        <v>598</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C49" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>165</v>
+      </c>
+      <c r="E49" t="s">
+        <v>599</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C50" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>165</v>
+      </c>
+      <c r="E50" t="s">
+        <v>592</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -4046,8 +4836,17 @@
       <c r="C51" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>166</v>
+      </c>
+      <c r="E51" t="s">
+        <v>566</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -4057,8 +4856,17 @@
       <c r="C52" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" t="s">
+        <v>603</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -4068,8 +4876,17 @@
       <c r="C53" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>166</v>
+      </c>
+      <c r="E53" t="s">
+        <v>378</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -4079,8 +4896,17 @@
       <c r="C54" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" t="s">
+        <v>604</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -4090,8 +4916,17 @@
       <c r="C55" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>166</v>
+      </c>
+      <c r="E55" t="s">
+        <v>605</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -4101,8 +4936,17 @@
       <c r="C56" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>166</v>
+      </c>
+      <c r="E56" t="s">
+        <v>606</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -4112,8 +4956,17 @@
       <c r="C57" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>166</v>
+      </c>
+      <c r="E57" t="s">
+        <v>607</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -4123,8 +4976,11 @@
       <c r="C58" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -4134,8 +4990,14 @@
       <c r="C59" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>168</v>
+      </c>
+      <c r="E59" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -4145,8 +5007,11 @@
       <c r="C60" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -4156,8 +5021,17 @@
       <c r="C61" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>170</v>
+      </c>
+      <c r="E61" t="s">
+        <v>566</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -4167,8 +5041,17 @@
       <c r="C62" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>170</v>
+      </c>
+      <c r="E62" t="s">
+        <v>609</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -4178,8 +5061,17 @@
       <c r="C63" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>170</v>
+      </c>
+      <c r="E63" t="s">
+        <v>610</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -4189,8 +5081,17 @@
       <c r="C64" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>170</v>
+      </c>
+      <c r="E64" t="s">
+        <v>611</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -4200,8 +5101,17 @@
       <c r="C65" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>170</v>
+      </c>
+      <c r="E65" t="s">
+        <v>612</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -4211,8 +5121,17 @@
       <c r="C66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>170</v>
+      </c>
+      <c r="E66" t="s">
+        <v>613</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -4222,8 +5141,17 @@
       <c r="C67" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>170</v>
+      </c>
+      <c r="E67" t="s">
+        <v>614</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -4233,8 +5161,17 @@
       <c r="C68" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>170</v>
+      </c>
+      <c r="E68" t="s">
+        <v>615</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>65</v>
       </c>
@@ -4244,8 +5181,17 @@
       <c r="C69" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>171</v>
+      </c>
+      <c r="E69" t="s">
+        <v>616</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -4255,8 +5201,17 @@
       <c r="C70" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>171</v>
+      </c>
+      <c r="E70" t="s">
+        <v>617</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -4266,8 +5221,17 @@
       <c r="C71" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>171</v>
+      </c>
+      <c r="E71" t="s">
+        <v>618</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>68</v>
       </c>
@@ -4277,8 +5241,17 @@
       <c r="C72" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>171</v>
+      </c>
+      <c r="E72" t="s">
+        <v>619</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>69</v>
       </c>
@@ -4288,8 +5261,17 @@
       <c r="C73" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>171</v>
+      </c>
+      <c r="E73" t="s">
+        <v>620</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -4299,8 +5281,17 @@
       <c r="C74" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>171</v>
+      </c>
+      <c r="E74" t="s">
+        <v>614</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -4310,8 +5301,17 @@
       <c r="C75" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>171</v>
+      </c>
+      <c r="E75" t="s">
+        <v>615</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>72</v>
       </c>
@@ -4321,8 +5321,11 @@
       <c r="C76" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -4332,8 +5335,11 @@
       <c r="C77" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -4343,8 +5349,11 @@
       <c r="C78" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>75</v>
       </c>
@@ -4354,8 +5363,17 @@
       <c r="C79" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>175</v>
+      </c>
+      <c r="E79" t="s">
+        <v>566</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -4365,8 +5383,17 @@
       <c r="C80" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>175</v>
+      </c>
+      <c r="E80" t="s">
+        <v>621</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -4376,8 +5403,17 @@
       <c r="C81" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
+        <v>175</v>
+      </c>
+      <c r="E81" t="s">
+        <v>622</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -4387,8 +5423,17 @@
       <c r="C82" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>175</v>
+      </c>
+      <c r="E82" t="s">
+        <v>623</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -4398,8 +5443,17 @@
       <c r="C83" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
+        <v>175</v>
+      </c>
+      <c r="E83" t="s">
+        <v>624</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -4409,8 +5463,17 @@
       <c r="C84" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>175</v>
+      </c>
+      <c r="E84" t="s">
+        <v>625</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -4420,8 +5483,17 @@
       <c r="C85" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>175</v>
+      </c>
+      <c r="E85" t="s">
+        <v>626</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>82</v>
       </c>
@@ -4431,8 +5503,17 @@
       <c r="C86" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>175</v>
+      </c>
+      <c r="E86" t="s">
+        <v>627</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>83</v>
       </c>
@@ -4442,8 +5523,17 @@
       <c r="C87" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
+        <v>175</v>
+      </c>
+      <c r="E87" t="s">
+        <v>628</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>84</v>
       </c>
@@ -4453,8 +5543,17 @@
       <c r="C88" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>175</v>
+      </c>
+      <c r="E88" t="s">
+        <v>629</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -4464,8 +5563,14 @@
       <c r="C89" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>176</v>
+      </c>
+      <c r="E89" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>86</v>
       </c>
@@ -4475,8 +5580,17 @@
       <c r="C90" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>177</v>
+      </c>
+      <c r="E90" t="s">
+        <v>630</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -4486,8 +5600,17 @@
       <c r="C91" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>177</v>
+      </c>
+      <c r="E91" t="s">
+        <v>631</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -4497,8 +5620,11 @@
       <c r="C92" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>89</v>
       </c>
@@ -4508,8 +5634,17 @@
       <c r="C93" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>632</v>
+      </c>
+      <c r="E93" t="s">
+        <v>633</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>90</v>
       </c>
@@ -4519,8 +5654,17 @@
       <c r="C94" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>634</v>
+      </c>
+      <c r="E94" t="s">
+        <v>635</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>91</v>
       </c>
@@ -4530,8 +5674,17 @@
       <c r="C95" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>636</v>
+      </c>
+      <c r="E95" t="s">
+        <v>637</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>92</v>
       </c>
@@ -4541,8 +5694,17 @@
       <c r="C96" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>180</v>
+      </c>
+      <c r="E96" t="s">
+        <v>566</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>93</v>
       </c>
@@ -4552,162 +5714,297 @@
       <c r="C97" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>180</v>
+      </c>
+      <c r="E97" t="s">
+        <v>638</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>94</v>
       </c>
       <c r="B98" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="C98" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>180</v>
+      </c>
+      <c r="E98" t="s">
+        <v>434</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>95</v>
       </c>
       <c r="B99" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="C99" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>180</v>
+      </c>
+      <c r="E99" t="s">
+        <v>644</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>96</v>
       </c>
       <c r="B100" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="C100" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>180</v>
+      </c>
+      <c r="E100" t="s">
+        <v>645</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>97</v>
       </c>
       <c r="B101" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="C101" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>180</v>
+      </c>
+      <c r="E101" t="s">
+        <v>646</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>98</v>
       </c>
       <c r="B102" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="C102" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
+        <v>180</v>
+      </c>
+      <c r="E102" t="s">
+        <v>647</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>99</v>
       </c>
       <c r="B103" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C103" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
+        <v>180</v>
+      </c>
+      <c r="E103" t="s">
+        <v>648</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>100</v>
       </c>
       <c r="B104" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C104" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104" t="s">
+        <v>180</v>
+      </c>
+      <c r="E104" t="s">
+        <v>639</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>101</v>
       </c>
       <c r="B105" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C105" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
+        <v>180</v>
+      </c>
+      <c r="E105" t="s">
+        <v>441</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C106" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
+        <v>180</v>
+      </c>
+      <c r="E106" t="s">
+        <v>442</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>103</v>
       </c>
       <c r="B107" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C107" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>180</v>
+      </c>
+      <c r="E107" t="s">
+        <v>443</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C108" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
+        <v>180</v>
+      </c>
+      <c r="E108" t="s">
+        <v>640</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C109" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
+        <v>180</v>
+      </c>
+      <c r="E109" t="s">
+        <v>641</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C110" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110" t="s">
+        <v>180</v>
+      </c>
+      <c r="E110" t="s">
+        <v>642</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>107</v>
       </c>
       <c r="B111" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C111" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D111" t="s">
+        <v>180</v>
+      </c>
+      <c r="E111" t="s">
+        <v>643</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>108</v>
       </c>
@@ -4717,8 +6014,11 @@
       <c r="C112" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D112" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>109</v>
       </c>
@@ -4728,8 +6028,11 @@
       <c r="C113" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>110</v>
       </c>
@@ -4739,8 +6042,17 @@
       <c r="C114" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
+        <v>183</v>
+      </c>
+      <c r="E114" t="s">
+        <v>456</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>111</v>
       </c>
@@ -4750,8 +6062,17 @@
       <c r="C115" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D115" t="s">
+        <v>183</v>
+      </c>
+      <c r="E115" t="s">
+        <v>457</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>112</v>
       </c>
@@ -4761,8 +6082,17 @@
       <c r="C116" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
+        <v>183</v>
+      </c>
+      <c r="E116" t="s">
+        <v>458</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>113</v>
       </c>
@@ -4772,8 +6102,17 @@
       <c r="C117" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
+        <v>183</v>
+      </c>
+      <c r="E117" t="s">
+        <v>649</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>114</v>
       </c>
@@ -4783,8 +6122,17 @@
       <c r="C118" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
+        <v>183</v>
+      </c>
+      <c r="E118" t="s">
+        <v>650</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>115</v>
       </c>
@@ -4794,8 +6142,17 @@
       <c r="C119" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
+        <v>183</v>
+      </c>
+      <c r="E119" t="s">
+        <v>461</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>116</v>
       </c>
@@ -4805,8 +6162,17 @@
       <c r="C120" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D120" t="s">
+        <v>184</v>
+      </c>
+      <c r="E120" t="s">
+        <v>651</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>117</v>
       </c>
@@ -4816,8 +6182,17 @@
       <c r="C121" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
+        <v>184</v>
+      </c>
+      <c r="E121" t="s">
+        <v>652</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>118</v>
       </c>
@@ -4827,8 +6202,17 @@
       <c r="C122" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
+        <v>184</v>
+      </c>
+      <c r="E122" t="s">
+        <v>653</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -4838,8 +6222,17 @@
       <c r="C123" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
+        <v>184</v>
+      </c>
+      <c r="E123" t="s">
+        <v>654</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>120</v>
       </c>
@@ -4849,8 +6242,17 @@
       <c r="C124" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
+        <v>184</v>
+      </c>
+      <c r="E124" t="s">
+        <v>655</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>121</v>
       </c>
@@ -4860,8 +6262,17 @@
       <c r="C125" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
+        <v>184</v>
+      </c>
+      <c r="E125" t="s">
+        <v>656</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>122</v>
       </c>
@@ -4871,8 +6282,17 @@
       <c r="C126" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
+        <v>184</v>
+      </c>
+      <c r="E126" t="s">
+        <v>657</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>123</v>
       </c>
@@ -4882,8 +6302,17 @@
       <c r="C127" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
+        <v>184</v>
+      </c>
+      <c r="E127" t="s">
+        <v>658</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>124</v>
       </c>
@@ -4893,8 +6322,17 @@
       <c r="C128" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
+        <v>184</v>
+      </c>
+      <c r="E128" t="s">
+        <v>592</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>125</v>
       </c>
@@ -4904,8 +6342,17 @@
       <c r="C129" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
+        <v>185</v>
+      </c>
+      <c r="E129" t="s">
+        <v>566</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>126</v>
       </c>
@@ -4915,8 +6362,17 @@
       <c r="C130" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
+        <v>185</v>
+      </c>
+      <c r="E130" t="s">
+        <v>659</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>127</v>
       </c>
@@ -4926,8 +6382,17 @@
       <c r="C131" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
+        <v>185</v>
+      </c>
+      <c r="E131" t="s">
+        <v>660</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>128</v>
       </c>
@@ -4937,8 +6402,17 @@
       <c r="C132" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
+        <v>185</v>
+      </c>
+      <c r="E132" t="s">
+        <v>661</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>129</v>
       </c>
@@ -4948,8 +6422,17 @@
       <c r="C133" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
+        <v>185</v>
+      </c>
+      <c r="E133" t="s">
+        <v>662</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>130</v>
       </c>
@@ -4959,8 +6442,17 @@
       <c r="C134" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D134" t="s">
+        <v>185</v>
+      </c>
+      <c r="E134" t="s">
+        <v>663</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>131</v>
       </c>
@@ -4970,8 +6462,17 @@
       <c r="C135" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D135" t="s">
+        <v>185</v>
+      </c>
+      <c r="E135" t="s">
+        <v>664</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>132</v>
       </c>
@@ -4981,8 +6482,17 @@
       <c r="C136" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
+        <v>185</v>
+      </c>
+      <c r="E136" t="s">
+        <v>665</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>133</v>
       </c>
@@ -4992,8 +6502,17 @@
       <c r="C137" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D137" t="s">
+        <v>185</v>
+      </c>
+      <c r="E137" t="s">
+        <v>666</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>134</v>
       </c>
@@ -5003,8 +6522,17 @@
       <c r="C138" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
+        <v>185</v>
+      </c>
+      <c r="E138" t="s">
+        <v>667</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>135</v>
       </c>
@@ -5014,8 +6542,17 @@
       <c r="C139" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
+        <v>185</v>
+      </c>
+      <c r="E139" t="s">
+        <v>668</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>136</v>
       </c>
@@ -5025,8 +6562,17 @@
       <c r="C140" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>185</v>
+      </c>
+      <c r="E140" t="s">
+        <v>592</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>137</v>
       </c>
@@ -5036,8 +6582,11 @@
       <c r="C141" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>139</v>
       </c>
@@ -5047,8 +6596,11 @@
       <c r="C142" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>140</v>
       </c>
@@ -5058,8 +6610,11 @@
       <c r="C143" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>141</v>
       </c>
@@ -5069,8 +6624,11 @@
       <c r="C144" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D144" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>142</v>
       </c>
@@ -5080,8 +6638,11 @@
       <c r="C145" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>143</v>
       </c>
@@ -5091,8 +6652,11 @@
       <c r="C146" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>144</v>
       </c>
@@ -5102,8 +6666,11 @@
       <c r="C147" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D147" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>145</v>
       </c>
@@ -5113,8 +6680,11 @@
       <c r="C148" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D148" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>146</v>
       </c>
@@ -5124,10 +6694,13 @@
       <c r="C149" t="b">
         <v>1</v>
       </c>
+      <c r="D149" t="s">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C149">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="E4:E9 E12:E15 D1:F1 C1:C149">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5139,7 +6712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5370D6F9-7760-C640-A095-DECD66441409}">
   <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -7184,7 +8757,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1 C1:C1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7203,22 +8776,22 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
     <col min="3" max="3" width="70" style="1" customWidth="1"/>
     <col min="4" max="4" width="44.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>323</v>
       </c>
     </row>
@@ -7226,7 +8799,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -7280,7 +8853,7 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>345</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -7291,7 +8864,7 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -7302,7 +8875,7 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -7380,7 +8953,7 @@
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -7434,7 +9007,7 @@
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -7520,7 +9093,7 @@
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -7630,7 +9203,7 @@
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="5">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -7692,7 +9265,7 @@
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="5">
         <v>9</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -7703,7 +9276,7 @@
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="5">
         <v>10</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -7714,7 +9287,7 @@
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="5">
         <v>12</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -7784,7 +9357,7 @@
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="5">
         <v>13</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -7846,7 +9419,7 @@
       <c r="A72" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="5" t="s">
         <v>401</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -7857,7 +9430,7 @@
       <c r="A73" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="5" t="s">
         <v>402</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -7868,7 +9441,7 @@
       <c r="A74" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="5" t="s">
         <v>403</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -7879,7 +9452,7 @@
       <c r="A75" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="5" t="s">
         <v>407</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -7965,7 +9538,7 @@
       <c r="A85" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B85" s="5" t="s">
         <v>417</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -7976,7 +9549,7 @@
       <c r="A86" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B86" s="5" t="s">
         <v>418</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -7987,7 +9560,7 @@
       <c r="A87" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="5" t="s">
         <v>419</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -7998,7 +9571,7 @@
       <c r="A88" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B88" s="5" t="s">
         <v>424</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -8009,7 +9582,7 @@
       <c r="A89" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="5" t="s">
         <v>426</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -8020,7 +9593,7 @@
       <c r="A90" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B90" s="5" t="s">
         <v>428</v>
       </c>
       <c r="C90" s="1" t="s">
@@ -8031,7 +9604,7 @@
       <c r="A91" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B91" s="5" t="s">
         <v>430</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -8042,7 +9615,7 @@
       <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="5" t="s">
         <v>431</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -8176,7 +9749,7 @@
       <c r="A108" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="6" t="s">
+      <c r="B108" s="5" t="s">
         <v>448</v>
       </c>
       <c r="C108" s="1" t="s">
@@ -8187,7 +9760,7 @@
       <c r="A109" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="5" t="s">
         <v>451</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -8198,7 +9771,7 @@
       <c r="A110" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B110" s="6" t="s">
+      <c r="B110" s="5" t="s">
         <v>453</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -8252,7 +9825,7 @@
       <c r="A116" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B116" s="6" t="s">
+      <c r="B116" s="5" t="s">
         <v>454</v>
       </c>
       <c r="C116" s="1" t="s">
@@ -8330,7 +9903,7 @@
       <c r="A125" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B125" s="6" t="s">
+      <c r="B125" s="5" t="s">
         <v>455</v>
       </c>
       <c r="C125" s="1" t="s">
@@ -8421,7 +9994,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor change to intro text, see email 2024-08-30
</commit_message>
<xml_diff>
--- a/inst/extdata/shiny_parameters.xlsx
+++ b/inst/extdata/shiny_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/shinycdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584388BF-5458-084C-B8C3-80CA0577BE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E867BFE-5D27-324A-B3F9-6CE7A800B107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="740" windowWidth="21340" windowHeight="18180" activeTab="1" xr2:uid="{76170439-9F00-B945-82EE-6E36AD1655CA}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{76170439-9F00-B945-82EE-6E36AD1655CA}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="2" r:id="rId1"/>
@@ -1494,10 +1494,6 @@
   </si>
   <si>
     <t>Overview</t>
-  </si>
-  <si>
-    <t>The Sacramento-San Joaquin Delta is the largest estuary on the west coast and the heart of California. The health and well-being of the Delta ecosystem and residents are deeply
-intertwined. The Delta Residents Survey research project was launched in 2023 by a collaborative group of university partners and California state agencies (California Sea Grant, University of California Davis, University of California Berkeley, Sacramento State University, Oregon State University, and the Delta Stewardship Council) as an effort to measure the well-being of Delta residents and understand how Delta communities are changing over time in response to regional social and environmental changes.</t>
   </si>
   <si>
     <t>p</t>
@@ -2167,6 +2163,9 @@
   </si>
   <si>
     <t>Other barrier. Please specify:</t>
+  </si>
+  <si>
+    <t>The Delta Residents Survey is the name of a social science study that seeks to measure the well-being of people who live in the Delta and to understand how these communities are changing over time in response to regional social and environmental changes. The project was launched in 2023 by a collaborative group of university partners—California Sea Grant, University of California Davis, University of California Berkeley, Sacramento State University and Oregon State University—and was funded by the Delta Stewardship Council. Over 2,200 Delta residents responded to the survey. This web app provides a way to explore the survey results.</t>
   </si>
 </sst>
 </file>
@@ -2255,7 +2254,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2283,36 +2282,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2648,8 +2617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A2E599-78C6-9D48-AFF2-88876341DCD3}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2664,10 +2633,10 @@
         <v>316</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>483</v>
@@ -2676,7 +2645,7 @@
         <v>186</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2702,10 +2671,10 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>485</v>
+        <v>680</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -2718,10 +2687,10 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2735,7 +2704,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2748,10 +2717,10 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2764,10 +2733,10 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2780,7 +2749,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -2793,10 +2762,10 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -2809,10 +2778,10 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -2825,7 +2794,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -2838,10 +2807,10 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>494</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -2853,13 +2822,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -2872,10 +2841,10 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -2888,10 +2857,10 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -2904,10 +2873,10 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -2920,10 +2889,10 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -2935,13 +2904,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -2954,10 +2923,10 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -2969,13 +2938,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -2988,10 +2957,10 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -3004,10 +2973,10 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -3020,10 +2989,10 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -3036,10 +3005,10 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -3051,13 +3020,13 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -3070,10 +3039,10 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -3085,13 +3054,13 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -3104,10 +3073,10 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -3120,10 +3089,10 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -3136,10 +3105,10 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -3152,10 +3121,10 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -3168,10 +3137,10 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -3183,13 +3152,13 @@
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F33" s="1"/>
     </row>
@@ -3202,10 +3171,10 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -3217,13 +3186,13 @@
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -3236,10 +3205,10 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F36" s="1"/>
     </row>
@@ -3252,10 +3221,10 @@
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F37" s="1"/>
     </row>
@@ -3268,10 +3237,10 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F38" s="1"/>
     </row>
@@ -3284,10 +3253,10 @@
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -3300,10 +3269,10 @@
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F40" s="1"/>
     </row>
@@ -3315,13 +3284,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F41" s="1"/>
     </row>
@@ -3334,10 +3303,10 @@
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F42" s="1"/>
     </row>
@@ -3350,10 +3319,10 @@
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F43" s="1"/>
     </row>
@@ -3365,13 +3334,13 @@
         <v>0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F44" s="1"/>
     </row>
@@ -3384,10 +3353,10 @@
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F45" s="1"/>
     </row>
@@ -3400,10 +3369,10 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F46" s="1"/>
     </row>
@@ -3416,10 +3385,10 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F47" s="1"/>
     </row>
@@ -3431,13 +3400,13 @@
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F48" s="1"/>
     </row>
@@ -3450,10 +3419,10 @@
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F49" s="1"/>
     </row>
@@ -3465,13 +3434,13 @@
         <v>0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F50" s="1"/>
     </row>
@@ -3484,7 +3453,7 @@
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>153</v>
@@ -3500,10 +3469,10 @@
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F52" s="1"/>
     </row>
@@ -3516,10 +3485,10 @@
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F53" s="1"/>
     </row>
@@ -3532,10 +3501,10 @@
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F54" s="1"/>
     </row>
@@ -3548,10 +3517,10 @@
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F55" s="1"/>
     </row>
@@ -3564,10 +3533,10 @@
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F56" s="1"/>
     </row>
@@ -3580,10 +3549,10 @@
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F57" s="1"/>
     </row>
@@ -3595,13 +3564,13 @@
         <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F58" s="1"/>
     </row>
@@ -3615,7 +3584,7 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F59" s="1"/>
     </row>
@@ -3628,10 +3597,10 @@
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F60" s="1"/>
     </row>
@@ -3644,10 +3613,10 @@
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F61" s="1"/>
     </row>
@@ -3660,10 +3629,10 @@
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F62" s="1"/>
     </row>
@@ -3676,10 +3645,10 @@
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F63" s="1"/>
     </row>
@@ -3692,10 +3661,10 @@
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F64" s="1"/>
     </row>
@@ -3708,10 +3677,10 @@
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F65" s="1"/>
     </row>
@@ -3725,7 +3694,7 @@
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F66" s="1"/>
     </row>
@@ -3738,10 +3707,10 @@
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F67" s="1"/>
     </row>
@@ -3754,10 +3723,10 @@
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F68" s="1"/>
     </row>
@@ -3771,7 +3740,7 @@
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F69" s="1"/>
     </row>
@@ -3784,10 +3753,10 @@
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F70" s="1"/>
     </row>
@@ -3800,10 +3769,10 @@
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F71" s="1"/>
     </row>
@@ -3816,10 +3785,10 @@
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F72" s="1"/>
     </row>
@@ -3844,7 +3813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B35F82-DAC3-AF45-8FCA-85CC06C5BE17}">
   <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B13" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -3867,13 +3836,13 @@
         <v>149</v>
       </c>
       <c r="D1" t="s">
+        <v>563</v>
+      </c>
+      <c r="E1" t="s">
         <v>564</v>
       </c>
-      <c r="E1" t="s">
-        <v>565</v>
-      </c>
       <c r="F1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3918,7 +3887,7 @@
         <v>158</v>
       </c>
       <c r="E4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>324</v>
@@ -3938,7 +3907,7 @@
         <v>158</v>
       </c>
       <c r="E5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>325</v>
@@ -3958,7 +3927,7 @@
         <v>158</v>
       </c>
       <c r="E6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>326</v>
@@ -3978,7 +3947,7 @@
         <v>158</v>
       </c>
       <c r="E7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>327</v>
@@ -3998,7 +3967,7 @@
         <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>328</v>
@@ -4018,7 +3987,7 @@
         <v>158</v>
       </c>
       <c r="E9" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>329</v>
@@ -4066,7 +4035,7 @@
         <v>161</v>
       </c>
       <c r="E12" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>330</v>
@@ -4086,7 +4055,7 @@
         <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>331</v>
@@ -4106,7 +4075,7 @@
         <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>332</v>
@@ -4126,7 +4095,7 @@
         <v>161</v>
       </c>
       <c r="E15" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>333</v>
@@ -4146,7 +4115,7 @@
         <v>161</v>
       </c>
       <c r="E16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>334</v>
@@ -4166,10 +4135,10 @@
         <v>161</v>
       </c>
       <c r="E17" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -4186,7 +4155,7 @@
         <v>161</v>
       </c>
       <c r="E18" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>336</v>
@@ -4206,7 +4175,7 @@
         <v>161</v>
       </c>
       <c r="E19" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>337</v>
@@ -4226,7 +4195,7 @@
         <v>161</v>
       </c>
       <c r="E20" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>338</v>
@@ -4246,7 +4215,7 @@
         <v>162</v>
       </c>
       <c r="E21" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>339</v>
@@ -4266,7 +4235,7 @@
         <v>162</v>
       </c>
       <c r="E22" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>340</v>
@@ -4286,7 +4255,7 @@
         <v>162</v>
       </c>
       <c r="E23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>341</v>
@@ -4306,7 +4275,7 @@
         <v>162</v>
       </c>
       <c r="E24" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>342</v>
@@ -4326,7 +4295,7 @@
         <v>162</v>
       </c>
       <c r="E25" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>343</v>
@@ -4346,7 +4315,7 @@
         <v>162</v>
       </c>
       <c r="E26" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>348</v>
@@ -4380,10 +4349,10 @@
         <v>164</v>
       </c>
       <c r="E28" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4400,7 +4369,7 @@
         <v>164</v>
       </c>
       <c r="E29" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>352</v>
@@ -4420,7 +4389,7 @@
         <v>164</v>
       </c>
       <c r="E30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>353</v>
@@ -4440,7 +4409,7 @@
         <v>164</v>
       </c>
       <c r="E31" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>354</v>
@@ -4460,7 +4429,7 @@
         <v>164</v>
       </c>
       <c r="E32" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>355</v>
@@ -4480,7 +4449,7 @@
         <v>164</v>
       </c>
       <c r="E33" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>356</v>
@@ -4500,7 +4469,7 @@
         <v>164</v>
       </c>
       <c r="E34" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>357</v>
@@ -4520,7 +4489,7 @@
         <v>164</v>
       </c>
       <c r="E35" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>358</v>
@@ -4540,7 +4509,7 @@
         <v>164</v>
       </c>
       <c r="E36" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>359</v>
@@ -4560,10 +4529,10 @@
         <v>164</v>
       </c>
       <c r="E37" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4580,7 +4549,7 @@
         <v>165</v>
       </c>
       <c r="E38" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>363</v>
@@ -4600,7 +4569,7 @@
         <v>165</v>
       </c>
       <c r="E39" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>364</v>
@@ -4620,7 +4589,7 @@
         <v>165</v>
       </c>
       <c r="E40" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>365</v>
@@ -4640,7 +4609,7 @@
         <v>165</v>
       </c>
       <c r="E41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>366</v>
@@ -4660,7 +4629,7 @@
         <v>165</v>
       </c>
       <c r="E42" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>367</v>
@@ -4680,7 +4649,7 @@
         <v>165</v>
       </c>
       <c r="E43" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>368</v>
@@ -4700,7 +4669,7 @@
         <v>165</v>
       </c>
       <c r="E44" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>369</v>
@@ -4720,7 +4689,7 @@
         <v>165</v>
       </c>
       <c r="E45" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>370</v>
@@ -4740,7 +4709,7 @@
         <v>165</v>
       </c>
       <c r="E46" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>371</v>
@@ -4780,7 +4749,7 @@
         <v>165</v>
       </c>
       <c r="E48" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>373</v>
@@ -4800,7 +4769,7 @@
         <v>165</v>
       </c>
       <c r="E49" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>374</v>
@@ -4820,7 +4789,7 @@
         <v>165</v>
       </c>
       <c r="E50" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>375</v>
@@ -4840,7 +4809,7 @@
         <v>166</v>
       </c>
       <c r="E51" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>324</v>
@@ -4860,7 +4829,7 @@
         <v>166</v>
       </c>
       <c r="E52" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>377</v>
@@ -4900,7 +4869,7 @@
         <v>166</v>
       </c>
       <c r="E54" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>379</v>
@@ -4920,7 +4889,7 @@
         <v>166</v>
       </c>
       <c r="E55" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>380</v>
@@ -4940,7 +4909,7 @@
         <v>166</v>
       </c>
       <c r="E56" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>381</v>
@@ -4960,7 +4929,7 @@
         <v>166</v>
       </c>
       <c r="E57" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>382</v>
@@ -4994,7 +4963,7 @@
         <v>168</v>
       </c>
       <c r="E59" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -5025,7 +4994,7 @@
         <v>170</v>
       </c>
       <c r="E61" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>330</v>
@@ -5045,7 +5014,7 @@
         <v>170</v>
       </c>
       <c r="E62" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>386</v>
@@ -5065,7 +5034,7 @@
         <v>170</v>
       </c>
       <c r="E63" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>387</v>
@@ -5085,7 +5054,7 @@
         <v>170</v>
       </c>
       <c r="E64" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>388</v>
@@ -5105,7 +5074,7 @@
         <v>170</v>
       </c>
       <c r="E65" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>389</v>
@@ -5125,7 +5094,7 @@
         <v>170</v>
       </c>
       <c r="E66" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>390</v>
@@ -5145,7 +5114,7 @@
         <v>170</v>
       </c>
       <c r="E67" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>391</v>
@@ -5165,7 +5134,7 @@
         <v>170</v>
       </c>
       <c r="E68" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>392</v>
@@ -5185,7 +5154,7 @@
         <v>171</v>
       </c>
       <c r="E69" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>395</v>
@@ -5205,7 +5174,7 @@
         <v>171</v>
       </c>
       <c r="E70" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>396</v>
@@ -5225,7 +5194,7 @@
         <v>171</v>
       </c>
       <c r="E71" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>397</v>
@@ -5245,7 +5214,7 @@
         <v>171</v>
       </c>
       <c r="E72" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>398</v>
@@ -5265,7 +5234,7 @@
         <v>171</v>
       </c>
       <c r="E73" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>399</v>
@@ -5285,7 +5254,7 @@
         <v>171</v>
       </c>
       <c r="E74" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>391</v>
@@ -5305,7 +5274,7 @@
         <v>171</v>
       </c>
       <c r="E75" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>392</v>
@@ -5367,7 +5336,7 @@
         <v>175</v>
       </c>
       <c r="E79" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>324</v>
@@ -5387,7 +5356,7 @@
         <v>175</v>
       </c>
       <c r="E80" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>408</v>
@@ -5407,10 +5376,10 @@
         <v>175</v>
       </c>
       <c r="E81" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -5427,7 +5396,7 @@
         <v>175</v>
       </c>
       <c r="E82" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>410</v>
@@ -5447,10 +5416,10 @@
         <v>175</v>
       </c>
       <c r="E83" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -5467,7 +5436,7 @@
         <v>175</v>
       </c>
       <c r="E84" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>412</v>
@@ -5487,10 +5456,10 @@
         <v>175</v>
       </c>
       <c r="E85" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -5507,7 +5476,7 @@
         <v>175</v>
       </c>
       <c r="E86" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>414</v>
@@ -5527,7 +5496,7 @@
         <v>175</v>
       </c>
       <c r="E87" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>415</v>
@@ -5547,7 +5516,7 @@
         <v>175</v>
       </c>
       <c r="E88" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>416</v>
@@ -5567,7 +5536,7 @@
         <v>176</v>
       </c>
       <c r="E89" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -5584,10 +5553,10 @@
         <v>177</v>
       </c>
       <c r="E90" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -5604,10 +5573,10 @@
         <v>177</v>
       </c>
       <c r="E91" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -5635,13 +5604,13 @@
         <v>1</v>
       </c>
       <c r="D93" t="s">
+        <v>631</v>
+      </c>
+      <c r="E93" t="s">
         <v>632</v>
       </c>
-      <c r="E93" t="s">
-        <v>633</v>
-      </c>
       <c r="F93" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5655,13 +5624,13 @@
         <v>1</v>
       </c>
       <c r="D94" t="s">
+        <v>633</v>
+      </c>
+      <c r="E94" t="s">
         <v>634</v>
       </c>
-      <c r="E94" t="s">
-        <v>635</v>
-      </c>
       <c r="F94" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -5675,13 +5644,13 @@
         <v>1</v>
       </c>
       <c r="D95" t="s">
+        <v>635</v>
+      </c>
+      <c r="E95" t="s">
         <v>636</v>
       </c>
-      <c r="E95" t="s">
-        <v>637</v>
-      </c>
       <c r="F95" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5698,7 +5667,7 @@
         <v>180</v>
       </c>
       <c r="E96" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>330</v>
@@ -5718,7 +5687,7 @@
         <v>180</v>
       </c>
       <c r="E97" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>433</v>
@@ -5758,7 +5727,7 @@
         <v>180</v>
       </c>
       <c r="E99" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>435</v>
@@ -5778,7 +5747,7 @@
         <v>180</v>
       </c>
       <c r="E100" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>436</v>
@@ -5798,7 +5767,7 @@
         <v>180</v>
       </c>
       <c r="E101" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>437</v>
@@ -5818,7 +5787,7 @@
         <v>180</v>
       </c>
       <c r="E102" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>438</v>
@@ -5838,7 +5807,7 @@
         <v>180</v>
       </c>
       <c r="E103" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>439</v>
@@ -5858,7 +5827,7 @@
         <v>180</v>
       </c>
       <c r="E104" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>440</v>
@@ -5938,7 +5907,7 @@
         <v>180</v>
       </c>
       <c r="E108" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>444</v>
@@ -5958,7 +5927,7 @@
         <v>180</v>
       </c>
       <c r="E109" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>445</v>
@@ -5978,7 +5947,7 @@
         <v>180</v>
       </c>
       <c r="E110" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>446</v>
@@ -5998,7 +5967,7 @@
         <v>180</v>
       </c>
       <c r="E111" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>447</v>
@@ -6106,7 +6075,7 @@
         <v>183</v>
       </c>
       <c r="E117" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>459</v>
@@ -6126,7 +6095,7 @@
         <v>183</v>
       </c>
       <c r="E118" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>460</v>
@@ -6166,7 +6135,7 @@
         <v>184</v>
       </c>
       <c r="E120" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>463</v>
@@ -6186,7 +6155,7 @@
         <v>184</v>
       </c>
       <c r="E121" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>464</v>
@@ -6206,7 +6175,7 @@
         <v>184</v>
       </c>
       <c r="E122" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>465</v>
@@ -6226,7 +6195,7 @@
         <v>184</v>
       </c>
       <c r="E123" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>466</v>
@@ -6246,7 +6215,7 @@
         <v>184</v>
       </c>
       <c r="E124" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>467</v>
@@ -6266,7 +6235,7 @@
         <v>184</v>
       </c>
       <c r="E125" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>468</v>
@@ -6286,7 +6255,7 @@
         <v>184</v>
       </c>
       <c r="E126" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>469</v>
@@ -6306,7 +6275,7 @@
         <v>184</v>
       </c>
       <c r="E127" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>470</v>
@@ -6326,10 +6295,10 @@
         <v>184</v>
       </c>
       <c r="E128" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6346,7 +6315,7 @@
         <v>185</v>
       </c>
       <c r="E129" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>330</v>
@@ -6366,7 +6335,7 @@
         <v>185</v>
       </c>
       <c r="E130" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>473</v>
@@ -6386,7 +6355,7 @@
         <v>185</v>
       </c>
       <c r="E131" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>474</v>
@@ -6406,7 +6375,7 @@
         <v>185</v>
       </c>
       <c r="E132" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>475</v>
@@ -6426,7 +6395,7 @@
         <v>185</v>
       </c>
       <c r="E133" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>476</v>
@@ -6446,7 +6415,7 @@
         <v>185</v>
       </c>
       <c r="E134" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>477</v>
@@ -6466,7 +6435,7 @@
         <v>185</v>
       </c>
       <c r="E135" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>478</v>
@@ -6486,7 +6455,7 @@
         <v>185</v>
       </c>
       <c r="E136" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>479</v>
@@ -6506,10 +6475,10 @@
         <v>185</v>
       </c>
       <c r="E137" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -6526,7 +6495,7 @@
         <v>185</v>
       </c>
       <c r="E138" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>480</v>
@@ -6546,7 +6515,7 @@
         <v>185</v>
       </c>
       <c r="E139" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>481</v>
@@ -6566,10 +6535,10 @@
         <v>185</v>
       </c>
       <c r="E140" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -6699,7 +6668,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E4:E9 E12:E15 D1:F1 C1:C149">
+  <conditionalFormatting sqref="D1:F1 C1:C149 E4:E9 E12:E15">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Changed main intro text, see email 2024-08-30
</commit_message>
<xml_diff>
--- a/inst/extdata/shiny_parameters.xlsx
+++ b/inst/extdata/shiny_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenjitomari/Documents/GitHub/shinycdrs/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E867BFE-5D27-324A-B3F9-6CE7A800B107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1153E413-8DA3-3F4A-9943-220A7DC90605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{76170439-9F00-B945-82EE-6E36AD1655CA}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{76170439-9F00-B945-82EE-6E36AD1655CA}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="2" r:id="rId1"/>
@@ -2618,7 +2618,7 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>